<commit_message>
ultimas modificaciones para el caso de uso
</commit_message>
<xml_diff>
--- a/artefacto_desarrollo_arq002.xlsx
+++ b/artefacto_desarrollo_arq002.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARCHIVOS_PERSONALES\VIDEO_ARQ_002\componentes_base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARCHIVOS_PERSONALES\CAMBIOS_A_REPO_ARQUETIPO_002\deinsoluciones-base-arq002-slim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FA50D2-5C28-460C-AB9E-F70A6CC01929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871B0B07-F014-40B0-9845-9861E62C3A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A12FCAE-AC36-4D74-BC93-581B6CD2A6BF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
   <si>
     <t>INFORMACION BASE</t>
   </si>
@@ -253,26 +253,121 @@
     <t>deinsoluciones-serverless</t>
   </si>
   <si>
-    <t>instrumentos-derivados-slim-nombre</t>
-  </si>
-  <si>
     <t>diario</t>
   </si>
   <si>
-    <t>tbl_instrumento_derivado_dia_nombre</t>
-  </si>
-  <si>
-    <t>sat_instrumento_derivado_dia_nombre</t>
-  </si>
-  <si>
-    <t>hub_operacion_derivado_nombre</t>
+    <r>
+      <t>instrumentos-derivados-slim-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nombre</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>tbl_instrumento_derivado_dia_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nombre</t>
+    </r>
+  </si>
+  <si>
+    <t>Fecha Ejecución</t>
+  </si>
+  <si>
+    <r>
+      <t>sat_instrumento_derivado_dia_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nombre</t>
+    </r>
+  </si>
+  <si>
+    <t>2025-04-24</t>
+  </si>
+  <si>
+    <r>
+      <t>hub_operacion_derivado_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nombre</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">se debe reemplazar el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nombre </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">por el nombre del participante aquí la variable antes de ser agregarda al archivo config.py debe ser algo como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>intrumendos-derivados-david</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +412,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -332,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -445,12 +548,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,6 +581,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -848,338 +972,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B092554-6C30-434B-A4AA-9519BC976F9D}">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="18" max="20" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="C9" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>54</v>
+      <c r="C27" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C31" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="33">
     <mergeCell ref="B2:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="C31:F31"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="C23:F23"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G6:R6"/>
+    <mergeCell ref="G18:R18"/>
+    <mergeCell ref="G23:R23"/>
+    <mergeCell ref="G25:R25"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C20:F20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" xr:uid="{207FD85B-65D5-4CB4-8C12-94710C89BAB7}"/>
+    <hyperlink ref="C29" r:id="rId1" xr:uid="{207FD85B-65D5-4CB4-8C12-94710C89BAB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -1191,7 +1400,7 @@
   <dimension ref="B4:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,30 +1410,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -1353,22 +1562,22 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1387,7 +1596,7 @@
   <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,50 +1613,50 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="I3" s="24" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="I3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="D4" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="I4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
+      <c r="J4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="I5" s="24" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="I5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">

</xml_diff>

<commit_message>
actualizacion de artefacto desarrollo
</commit_message>
<xml_diff>
--- a/artefacto_desarrollo_arq002.xlsx
+++ b/artefacto_desarrollo_arq002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARCHIVOS_PERSONALES\CAMBIOS_A_REPO_ARQUETIPO_002\deinsoluciones-base-arq002-slim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871B0B07-F014-40B0-9845-9861E62C3A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ECC9AD-1DB1-47B8-B935-0454EC17042C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A12FCAE-AC36-4D74-BC93-581B6CD2A6BF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
   <si>
     <t>INFORMACION BASE</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>Nombre Archivo:</t>
-  </si>
-  <si>
-    <t>instrumentos-derivados.parquet</t>
   </si>
   <si>
     <t>DETALLE PARTICION</t>
@@ -360,6 +357,32 @@
         <scheme val="minor"/>
       </rPr>
       <t>intrumendos-derivados-david</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>instrumentos-derivados-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nombre</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.parquet</t>
     </r>
   </si>
 </sst>
@@ -586,6 +609,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,42 +653,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -975,7 +998,7 @@
   <dimension ref="B2:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,36 +1009,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -1025,326 +1048,340 @@
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="C6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="C9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="C15" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
+      <c r="C18" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+        <v>73</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
+      <c r="C23" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+        <v>73</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="22"/>
@@ -1352,12 +1389,20 @@
       <c r="F31" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
+  <mergeCells count="34">
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G6:R6"/>
+    <mergeCell ref="G18:R18"/>
+    <mergeCell ref="G23:R23"/>
+    <mergeCell ref="G25:R25"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G15:R15"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C8:F8"/>
@@ -1374,18 +1419,11 @@
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G6:R6"/>
-    <mergeCell ref="G18:R18"/>
-    <mergeCell ref="G23:R23"/>
-    <mergeCell ref="G25:R25"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29" r:id="rId1" xr:uid="{207FD85B-65D5-4CB4-8C12-94710C89BAB7}"/>
@@ -1422,7 +1460,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -1563,7 +1601,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -1631,7 +1669,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
@@ -1639,7 +1677,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>

</xml_diff>